<commit_message>
feat(pagination): usePagination hook for better paginate
</commit_message>
<xml_diff>
--- a/public/templates/template_kelas.xlsx
+++ b/public/templates/template_kelas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\JS\projects\TEFA\K-NEKt\next-k-nekt\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71C4ACFB-7E6F-42FE-B84C-76CFA43A3653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C53AC-BD42-47AC-840C-D569BABA2B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{723E451C-E063-473B-9F8A-1C6C1AFB8D5F}"/>
   </bookViews>
@@ -31,12 +31,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Kelas</t>
   </si>
   <si>
-    <t>(Contoh: XI Otomotif 2)</t>
+    <t>PETUNJUK</t>
+  </si>
+  <si>
+    <t>Format yang benar: XI (Menggunakan romawi) Nama kelas + No kelas (Contoh: OTOMOTIF 2)</t>
+  </si>
+  <si>
+    <t>Contoh lengkap: XI OTOMOTIF 2</t>
+  </si>
+  <si>
+    <t>(Contoh: XI OTOMOTIF 2)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +417,7 @@
   <cols>
     <col min="1" max="1" width="24.26953125" customWidth="1"/>
     <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="56.36328125" customWidth="1"/>
+    <col min="4" max="4" width="87.6328125" customWidth="1"/>
     <col min="5" max="5" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -422,14 +431,24 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
       <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H12" s="1"/>

</xml_diff>